<commit_message>
bgbgr Co-authored-by: siddharth rapol <Siddharth-HACKER@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/public/existing_data.xlsx
+++ b/public/existing_data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
-    <sheet r:id="rId2" sheetId="2" name="Sheet2"/>
-    <sheet r:id="rId3" sheetId="3" name="Sheet3"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Sheet2" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Sheet3" state="visible" r:id="rId6"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>studentname</t>
   </si>
@@ -115,20 +115,106 @@
   </si>
   <si>
     <t>9959848004</t>
+  </si>
+  <si>
+    <t>gdgdfdg</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>gdg</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>2024-02-02</t>
+  </si>
+  <si>
+    <t>3rd class</t>
+  </si>
+  <si>
+    <t>fgdffdffdsfsd</t>
+  </si>
+  <si>
+    <t>dfsfs</t>
+  </si>
+  <si>
+    <t>645654654654</t>
+  </si>
+  <si>
+    <t>5646456654</t>
+  </si>
+  <si>
+    <t>6456546546</t>
+  </si>
+  <si>
+    <t>gfdg</t>
+  </si>
+  <si>
+    <t>654</t>
+  </si>
+  <si>
+    <t>2024-02-13</t>
+  </si>
+  <si>
+    <t>LKG</t>
+  </si>
+  <si>
+    <t>65645</t>
+  </si>
+  <si>
+    <t>645645</t>
+  </si>
+  <si>
+    <t>655464564564</t>
+  </si>
+  <si>
+    <t>6456456546</t>
+  </si>
+  <si>
+    <t>6456456456</t>
+  </si>
+  <si>
+    <t>jbkdsjok</t>
+  </si>
+  <si>
+    <t>hfghgf</t>
+  </si>
+  <si>
+    <t>756</t>
+  </si>
+  <si>
+    <t>2024-02-05</t>
+  </si>
+  <si>
+    <t>76756756</t>
+  </si>
+  <si>
+    <t>756756</t>
+  </si>
+  <si>
+    <t>424554654645</t>
+  </si>
+  <si>
+    <t>6465465645</t>
+  </si>
+  <si>
+    <t>6546456546</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,23 +237,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -461,138 +544,241 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="12" width="13.576428571428572" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="18.75" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="18.75" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="18.75" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -605,11 +791,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -620,11 +806,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>